<commit_message>
need to finish b1, start b2
</commit_message>
<xml_diff>
--- a/Assignment 1/Assignment 1.xlsx
+++ b/Assignment 1/Assignment 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\raeedh\school\COMPENG4DM4\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDBDE19-C95E-4E9B-84DF-A3FCBFE9135A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7397966-A427-4405-81A3-6666FFDDC827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="43">
   <si>
     <t>4DM4 Assignment #1, Timing for Basic RISC 7-stage  pipeline</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -143,6 +143,36 @@
   </si>
   <si>
     <t>**forward R0 (ID** to **IF) in cc5</t>
+  </si>
+  <si>
+    <t>LD Ra,(0)R0</t>
+  </si>
+  <si>
+    <t>LD Rb,(16)R0</t>
+  </si>
+  <si>
+    <t>ADD Ra,Ra,Rb</t>
+  </si>
+  <si>
+    <t>SD (0)R0,Ra</t>
+  </si>
+  <si>
+    <t>LD Rd,(48)R0</t>
+  </si>
+  <si>
+    <t>XOR Rd,Rd,Rd</t>
+  </si>
+  <si>
+    <t>SD (48)R0,Rd</t>
+  </si>
+  <si>
+    <t>ROT.L Rd,Rd,#16</t>
+  </si>
+  <si>
+    <t>*forward Rb (MEM2* to *EX) in cc7</t>
+  </si>
+  <si>
+    <t>*MEM1</t>
   </si>
 </sst>
 </file>
@@ -308,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +368,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3738,15 +3769,15 @@
   </sheetPr>
   <dimension ref="B2:AF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.375" customWidth="1"/>
     <col min="2" max="2" width="28.125" customWidth="1"/>
-    <col min="3" max="32" width="8.75" customWidth="1"/>
+    <col min="3" max="32" width="8.625" customWidth="1"/>
     <col min="33" max="74" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3932,7 +3963,7 @@
     </row>
     <row r="6" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>4</v>
@@ -3943,21 +3974,19 @@
       <c r="E6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="13" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="J6" s="9"/>
       <c r="L6" s="9"/>
       <c r="N6" s="21"/>
       <c r="P6" s="9"/>
@@ -3980,7 +4009,7 @@
     </row>
     <row r="7" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
@@ -3989,27 +4018,25 @@
       <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="15" t="s">
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>9</v>
+      <c r="I7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>32</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4033,35 +4060,37 @@
     </row>
     <row r="8" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="9" t="s">
+      <c r="I8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
@@ -4084,36 +4113,38 @@
     </row>
     <row r="9" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="K9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
@@ -4135,37 +4166,43 @@
     </row>
     <row r="10" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="15" t="s">
-        <v>31</v>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="I10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="13" t="s">
+      <c r="P10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="9"/>
+      <c r="Q10" s="13"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
       <c r="T10" s="9"/>
@@ -4183,22 +4220,44 @@
       <c r="AF10" s="9"/>
     </row>
     <row r="11" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
@@ -4216,7 +4275,9 @@
       <c r="AF11" s="9"/>
     </row>
     <row r="12" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
+      <c r="B12" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -4225,16 +4286,36 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
+      <c r="K12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -4249,7 +4330,9 @@
       <c r="AF12" s="9"/>
     </row>
     <row r="13" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
+      <c r="B13" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -4259,12 +4342,24 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
+      <c r="L13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
@@ -4282,7 +4377,9 @@
       <c r="AF13" s="9"/>
     </row>
     <row r="14" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -4315,7 +4412,9 @@
       <c r="AF14" s="9"/>
     </row>
     <row r="15" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -4330,7 +4429,9 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="Q15" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
       <c r="T15" s="13"/>
@@ -4348,7 +4449,9 @@
       <c r="AF15" s="9"/>
     </row>
     <row r="16" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -4562,7 +4665,9 @@
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+      <c r="R22" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
@@ -4679,13 +4784,27 @@
     </row>
     <row r="26" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -4696,10 +4815,10 @@
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>

</xml_diff>

<commit_message>
add b1 to report
</commit_message>
<xml_diff>
--- a/Assignment 1/Assignment 1.xlsx
+++ b/Assignment 1/Assignment 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\raeedh\school\COMPENG4DM4\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3893A5CD-23F8-46F4-A401-0C3A7DA68517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937597C4-6B0C-4E1D-821F-436B87A93F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="47">
   <si>
     <t>4DM4 Assignment #1, Timing for Basic RISC 7-stage  pipeline</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>*MEM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">but </t>
   </si>
   <si>
     <t>*forward Rd (MEM2* to *EX) in cc14</t>
@@ -3812,7 +3809,7 @@
   <dimension ref="B2:AF41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4166,10 +4163,10 @@
       <c r="G9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="23" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="13" t="s">
@@ -4188,7 +4185,7 @@
         <v>10</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
@@ -4219,22 +4216,22 @@
       <c r="G10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="14" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="N10" s="17" t="s">
@@ -4272,10 +4269,10 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -4287,7 +4284,7 @@
       <c r="L11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="N11" s="13" t="s">
@@ -4303,7 +4300,7 @@
         <v>10</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
@@ -4338,16 +4335,16 @@
       <c r="L12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="M12" s="14" t="s">
         <v>12</v>
       </c>
       <c r="N12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="P12" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Q12" s="24" t="s">
@@ -4391,16 +4388,16 @@
       <c r="L13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="14" t="s">
         <v>12</v>
       </c>
       <c r="N13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="Q13" s="25" t="s">
@@ -4419,7 +4416,7 @@
         <v>10</v>
       </c>
       <c r="V13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
@@ -4446,16 +4443,16 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="14" t="s">
         <v>12</v>
       </c>
       <c r="N14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="P14" s="14" t="s">
         <v>12</v>
       </c>
       <c r="Q14" s="9" t="s">
@@ -4467,7 +4464,7 @@
       <c r="S14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="T14" s="19" t="s">
+      <c r="T14" s="20" t="s">
         <v>12</v>
       </c>
       <c r="U14" s="15" t="s">
@@ -4480,7 +4477,7 @@
         <v>10</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y14" s="9"/>
       <c r="Z14" s="9"/>
@@ -4507,10 +4504,10 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="9" t="s">
+      <c r="O15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="P15" s="14" t="s">
         <v>12</v>
       </c>
       <c r="Q15" s="9" t="s">
@@ -4522,13 +4519,13 @@
       <c r="S15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="T15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="U15" s="9" t="s">
+      <c r="U15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="V15" s="18" t="s">
+      <c r="V15" s="16" t="s">
         <v>12</v>
       </c>
       <c r="W15" s="26" t="s">
@@ -4575,13 +4572,13 @@
       <c r="S16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="T16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="U16" s="9" t="s">
+      <c r="U16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="V16" s="9" t="s">
+      <c r="V16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="W16" s="25" t="s">

</xml_diff>